<commit_message>
0.1.1 Release - Fixed a bug in which assertions were not being checked if a question/prompt was not relevant. - Added character escaping for usage of ':' in literal strings. An assertion string such as '777: 1234' no longer triggers a bug where XformTest thinks that '777' is an assertion field (e.g. value assertion, relevant assertion). - Added necessary requirement that every answerable question prompt not marked as require  must at the very least have include a value assertion. - Via addition of requirement of value assertion for answerable questions, related bugs were fixed. - Fixed bug where relevant assertion was sometimes not working correctly; either when assertion was 'relevant: false' but was true, or 'relevant: true' but was false. - Added 'n/a character' '.'. If putting '.' in the xform-test column, it is the same as leaving the column empty; stating that there are no assertions.
</commit_message>
<xml_diff>
--- a/test/static/XformTest/input/XformTest1.xlsx
+++ b/test/static/XformTest/input/XformTest1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28260" tabRatio="495"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="495"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -566,12 +566,6 @@
     <t>[636, 444]</t>
   </si>
   <si>
-    <t>[252: 123-636&amp;#x0a;, 777: 999-444&amp;#x0a;]</t>
-  </si>
-  <si>
-    <t>252: 123-636&amp;#x0a;777: 999-444&amp;#x0a;</t>
-  </si>
-  <si>
     <t>bind::xtest-linearAssert</t>
   </si>
   <si>
@@ -591,6 +585,12 @@
   </si>
   <si>
     <t>value: Country, relevant: 1</t>
+  </si>
+  <si>
+    <t>[252\: 123-636&amp;#x0a;, 777\: 999-444&amp;#x0a;]</t>
+  </si>
+  <si>
+    <t>252\: 123-636&amp;#x0a;777\: 999-444&amp;#x0a;</t>
   </si>
 </sst>
 </file>
@@ -676,11 +676,41 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="152">
+  <cellStyleXfs count="162">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1179,7 +1209,7 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="152">
+  <cellStyles count="162">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -1255,6 +1285,11 @@
     <cellStyle name="Followed Hyperlink" xfId="147" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="149" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="151" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="153" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="155" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="157" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="159" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="161" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1330,6 +1365,11 @@
     <cellStyle name="Hyperlink" xfId="146" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="148" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="150" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="152" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="154" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="156" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="158" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="160" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2 2" xfId="1"/>
   </cellStyles>
@@ -1781,10 +1821,10 @@
   <dimension ref="A1:N81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" zoomScalePageLayoutView="175" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomRight" activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.6640625" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0"/>
@@ -1845,7 +1885,7 @@
         <v>61</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="13" customHeight="1">
@@ -1868,7 +1908,7 @@
         <v>160</v>
       </c>
       <c r="N2" s="12" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="13" customHeight="1">
@@ -1885,7 +1925,7 @@
         <v>112</v>
       </c>
       <c r="N3" s="12" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="13" customHeight="1">
@@ -1905,7 +1945,7 @@
         <v>114</v>
       </c>
       <c r="N4" s="12" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="13" customHeight="1">
@@ -1922,7 +1962,7 @@
         <v>27</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>13</v>
@@ -1931,7 +1971,7 @@
         <v>115</v>
       </c>
       <c r="N5" s="12" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="13" customHeight="1">
@@ -1948,7 +1988,7 @@
         <v>161</v>
       </c>
       <c r="N6" s="12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="13" customHeight="1">
@@ -1967,10 +2007,7 @@
       <c r="K7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N7" s="13">
-        <f ca="1">TODAY()</f>
-        <v>43391</v>
-      </c>
+      <c r="N7" s="13"/>
     </row>
     <row r="8" spans="1:14" ht="13" customHeight="1">
       <c r="A8" s="1" t="s">
@@ -1997,7 +2034,7 @@
         <v>29</v>
       </c>
       <c r="N9" s="12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="13" customHeight="1">
@@ -2026,7 +2063,7 @@
         <v>163</v>
       </c>
       <c r="N10" s="12" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="11" spans="1:14" s="4" customFormat="1" ht="13" customHeight="1">
@@ -2050,7 +2087,7 @@
       </c>
       <c r="M11" s="1"/>
       <c r="N11" s="12" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="12" spans="1:14" s="4" customFormat="1" ht="13" customHeight="1">
@@ -2172,7 +2209,7 @@
       </c>
       <c r="M16" s="5"/>
       <c r="N16" s="12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="13" customHeight="1">
@@ -2186,7 +2223,7 @@
         <v>44</v>
       </c>
       <c r="N17" s="12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="13" customHeight="1">
@@ -2201,7 +2238,7 @@
         <v>1</v>
       </c>
       <c r="N18" s="12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="13" customHeight="1">
@@ -2264,7 +2301,7 @@
       </c>
       <c r="C22" s="6"/>
       <c r="N22" s="12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="13" customHeight="1">
@@ -2279,7 +2316,7 @@
         <v>75</v>
       </c>
       <c r="N23" s="12" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="13" customHeight="1">
@@ -2291,7 +2328,7 @@
       </c>
       <c r="C24" s="6"/>
       <c r="N24" s="12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="13" customHeight="1">
@@ -2333,7 +2370,7 @@
         <v>86</v>
       </c>
       <c r="N27" s="12" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="13" customHeight="1">
@@ -2347,7 +2384,7 @@
         <v>1</v>
       </c>
       <c r="N28" s="12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="13" customHeight="1">
@@ -2361,7 +2398,7 @@
         <v>78</v>
       </c>
       <c r="N29" s="12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="13" customHeight="1">
@@ -2389,7 +2426,7 @@
         <v>87</v>
       </c>
       <c r="N31" s="12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="13" customHeight="1">
@@ -2409,7 +2446,7 @@
         <v>90</v>
       </c>
       <c r="N32" s="12" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="13" customHeight="1">
@@ -2469,7 +2506,7 @@
         <v>80</v>
       </c>
       <c r="N35" s="12" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="13" customHeight="1">
@@ -2489,7 +2526,7 @@
         <v>56</v>
       </c>
       <c r="N36" s="12" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="13" customHeight="1">
@@ -2506,7 +2543,7 @@
         <v>101</v>
       </c>
       <c r="N37" s="12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="38" spans="1:14" ht="13" customHeight="1">
@@ -2614,7 +2651,7 @@
       <c r="D42" s="4"/>
       <c r="F42" s="4"/>
       <c r="N42" s="12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="43" spans="1:14" s="5" customFormat="1" ht="13" customHeight="1">
@@ -2630,7 +2667,7 @@
       <c r="D43" s="4"/>
       <c r="F43" s="4"/>
       <c r="N43" s="12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="44" spans="1:14" s="5" customFormat="1" ht="13" customHeight="1">
@@ -2646,7 +2683,7 @@
       <c r="D44" s="4"/>
       <c r="F44" s="4"/>
       <c r="N44" s="12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="45" spans="1:14" s="5" customFormat="1" ht="13" customHeight="1">
@@ -2662,7 +2699,7 @@
       <c r="D45" s="4"/>
       <c r="F45" s="4"/>
       <c r="N45" s="12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="46" spans="1:14" s="5" customFormat="1" ht="13" customHeight="1">
@@ -2678,7 +2715,7 @@
       <c r="D46" s="4"/>
       <c r="F46" s="4"/>
       <c r="N46" s="12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="50" spans="3:3" ht="13" customHeight="1">

</xml_diff>